<commit_message>
pensare al modello fenditura
</commit_message>
<xml_diff>
--- a/20240509micoonde/dati_microonde_2.xlsx
+++ b/20240509micoonde/dati_microonde_2.xlsx
@@ -60,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -70,13 +70,6 @@
     <font>
       <sz val="11.000000"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11.000000"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -108,13 +101,12 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2285,62 +2277,14 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-    </row>
-    <row r="35">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-    </row>
-    <row r="36">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-    </row>
-    <row r="37">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-    </row>
-    <row r="38">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-    </row>
-    <row r="39">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-    </row>
-    <row r="40">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-    </row>
-    <row r="41">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-    </row>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -2359,6 +2303,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="13.875"/>
     <col customWidth="1" min="4" max="5" width="13.6640625"/>
     <col customWidth="1" min="6" max="6" width="6.77734375"/>
   </cols>
@@ -2392,7 +2337,7 @@
         <v>48.799999999999997</v>
       </c>
       <c r="D2" s="3">
-        <f>B2-C2</f>
+        <f t="shared" ref="D2:D9" si="1">B2-C2</f>
         <v>51.200000000000003</v>
       </c>
       <c r="E2" s="4">
@@ -2410,7 +2355,7 @@
         <v>47.299999999999997</v>
       </c>
       <c r="D3" s="3">
-        <f>B3-C3</f>
+        <f t="shared" si="1"/>
         <v>52.700000000000003</v>
       </c>
       <c r="E3" s="4">
@@ -2428,7 +2373,7 @@
         <v>45.899999999999999</v>
       </c>
       <c r="D4" s="3">
-        <f>B4-C4</f>
+        <f t="shared" si="1"/>
         <v>54.100000000000001</v>
       </c>
       <c r="E4" s="4">
@@ -2446,7 +2391,7 @@
         <v>44.5</v>
       </c>
       <c r="D5" s="3">
-        <f>B5-C5</f>
+        <f t="shared" si="1"/>
         <v>55.5</v>
       </c>
       <c r="E5" s="4">
@@ -2464,7 +2409,7 @@
         <v>43</v>
       </c>
       <c r="D6" s="3">
-        <f>B6-C6</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="E6" s="4">
@@ -2482,7 +2427,7 @@
         <v>41.5</v>
       </c>
       <c r="D7" s="3">
-        <f>B7-C7</f>
+        <f t="shared" si="1"/>
         <v>58.5</v>
       </c>
       <c r="E7" s="4">
@@ -2500,7 +2445,7 @@
         <v>40.100000000000001</v>
       </c>
       <c r="D8" s="3">
-        <f>B8-C8</f>
+        <f t="shared" si="1"/>
         <v>59.899999999999999</v>
       </c>
       <c r="E8" s="4">
@@ -2518,7 +2463,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="D9" s="3">
-        <f>B9-C9</f>
+        <f t="shared" si="1"/>
         <v>61.299999999999997</v>
       </c>
       <c r="E9" s="4">
@@ -2536,7 +2481,7 @@
         <v>37.200000000000003</v>
       </c>
       <c r="D10" s="3">
-        <f>B10-C10</f>
+        <f t="shared" ref="D10:D23" si="2">B10-C10</f>
         <v>62.799999999999997</v>
       </c>
       <c r="E10" s="4">
@@ -2554,7 +2499,7 @@
         <v>35.799999999999997</v>
       </c>
       <c r="D11" s="3">
-        <f>B11-C11</f>
+        <f t="shared" si="2"/>
         <v>64.200000000000003</v>
       </c>
       <c r="E11" s="4">
@@ -2572,7 +2517,7 @@
         <v>34.5</v>
       </c>
       <c r="D12" s="3">
-        <f>B12-C12</f>
+        <f t="shared" si="2"/>
         <v>65.5</v>
       </c>
       <c r="E12" s="4">
@@ -2590,7 +2535,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="3">
-        <f>B13-C13</f>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="E13" s="4">
@@ -2608,7 +2553,7 @@
         <v>31.5</v>
       </c>
       <c r="D14" s="3">
-        <f>B14-C14</f>
+        <f t="shared" si="2"/>
         <v>68.5</v>
       </c>
       <c r="E14" s="4">
@@ -2626,7 +2571,7 @@
         <v>30.100000000000001</v>
       </c>
       <c r="D15" s="3">
-        <f>B15-C15</f>
+        <f t="shared" si="2"/>
         <v>69.900000000000006</v>
       </c>
       <c r="E15" s="4">
@@ -2644,7 +2589,7 @@
         <v>28.600000000000001</v>
       </c>
       <c r="D16" s="3">
-        <f>B16-C16</f>
+        <f t="shared" si="2"/>
         <v>71.400000000000006</v>
       </c>
       <c r="E16" s="4">
@@ -2662,7 +2607,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="3">
-        <f>B17-C17</f>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="E17" s="4">
@@ -2680,7 +2625,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="3">
-        <f>B18-C18</f>
+        <f t="shared" si="2"/>
         <v>49.599999999999994</v>
       </c>
       <c r="E18" s="4">
@@ -2698,7 +2643,7 @@
         <v>50</v>
       </c>
       <c r="D19" s="3">
-        <f>B19-C19</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="E19" s="4">
@@ -2716,7 +2661,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="3">
-        <f>B20-C20</f>
+        <f t="shared" si="2"/>
         <v>46.5</v>
       </c>
       <c r="E20" s="4">
@@ -2734,7 +2679,7 @@
         <v>50</v>
       </c>
       <c r="D21" s="3">
-        <f>B21-C21</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="E21" s="4">
@@ -2752,7 +2697,7 @@
         <v>50</v>
       </c>
       <c r="D22" s="3">
-        <f>B22-C22</f>
+        <f t="shared" si="2"/>
         <v>43.599999999999994</v>
       </c>
       <c r="E22" s="4">
@@ -2770,7 +2715,7 @@
         <v>50</v>
       </c>
       <c r="D23" s="3">
-        <f>B23-C23</f>
+        <f t="shared" si="2"/>
         <v>33.900000000000006</v>
       </c>
       <c r="E23" s="4">
@@ -2793,7 +2738,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="100" workbookViewId="0">
       <selection activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2807,345 +2752,400 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>100</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>50</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>20</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="C3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
         <v>25</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>22</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="C4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
         <v>30</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="C5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
         <v>35</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>106</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="C6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
         <v>40</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>176</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="5"/>
-      <c r="C7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
         <v>45</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>180</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
         <v>50</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>125</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="C9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
         <v>55</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>26</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="C10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1">
         <v>60</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>118</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="11">
-      <c r="C11">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
         <v>65</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>270</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="12">
-      <c r="C12">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1">
         <v>70</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>284</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
         <v>75</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>116</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1">
         <v>80</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>17</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="C15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1">
         <v>85</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>178</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1">
         <v>90</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>317</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="17">
-      <c r="C17">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1">
         <v>95</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>225</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="18">
-      <c r="C18">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1">
         <v>100</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>37</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1">
         <v>105</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>75</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1">
         <v>110</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>286</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1">
         <v>115</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>305</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="22">
-      <c r="C22">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1">
         <v>120</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>172</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1">
         <v>125</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>40</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1">
         <v>130</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>115</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1">
         <v>135</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>190</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="26">
-      <c r="C26">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1">
         <v>140</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>196</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1">
         <v>145</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>135</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1">
         <v>150</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>58</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1">
         <v>155</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>28</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1">
         <v>160</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>19</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>